<commit_message>
Alter task to get endpoint
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t xml:space="preserve">Меню</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Основное меню</t>
+    <t xml:space="preserve">-МЕНЮ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основное меню=yes</t>
   </si>
   <si>
     <t xml:space="preserve">Холодные закуски</t>
@@ -274,7 +274,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Altered objects comparison etc
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t xml:space="preserve">Меню--</t>
+    <t xml:space="preserve">Меню</t>
   </si>
   <si>
     <t xml:space="preserve">Основное меню</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
   </si>
   <si>
-    <t xml:space="preserve">Виски</t>
+    <t xml:space="preserve">Виски </t>
   </si>
   <si>
     <t xml:space="preserve">Для интересных бесед</t>
@@ -274,7 +274,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>